<commit_message>
Update 11_v01_PracticeCharacterizations PLACE HOLDER.xlsx
</commit_message>
<xml_diff>
--- a/2024-05-04to05-10 (A5) C384400 NASA/02_CASimportExport/11_v01_PracticeCharacterizations PLACE HOLDER.xlsx
+++ b/2024-05-04to05-10 (A5) C384400 NASA/02_CASimportExport/11_v01_PracticeCharacterizations PLACE HOLDER.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PietervanZyl\Documents\GitHub\CMMITools\2021-04-12to04-16 (A5) C53517 SoftMARS\02_CASimportExport\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pwjva\Documents\GitHub\CMMITools\2024-05-04to05-10 (A5) C384400 NASA\02_CASimportExport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{921286F7-2E2D-4070-B22A-B49DBEA2AD23}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{331CB4CC-CFD0-4F8D-9D41-FF056B012AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Staged Roll-Up" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="64">
   <si>
     <t>Level 5</t>
   </si>
@@ -89,13 +89,91 @@
     <t>Level 1</t>
   </si>
   <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>1.3</t>
+  </si>
+  <si>
     <t>Level 2</t>
+  </si>
+  <si>
+    <t>2.1</t>
+  </si>
+  <si>
+    <t>2.2</t>
+  </si>
+  <si>
+    <t>2.3</t>
+  </si>
+  <si>
+    <t>2.4</t>
+  </si>
+  <si>
+    <t>2.5</t>
+  </si>
+  <si>
+    <t>2.6</t>
+  </si>
+  <si>
+    <t>2.7</t>
+  </si>
+  <si>
+    <t>2.8</t>
   </si>
   <si>
     <t>Level 3</t>
   </si>
   <si>
+    <t>3.1</t>
+  </si>
+  <si>
+    <t>3.2</t>
+  </si>
+  <si>
+    <t>3.3</t>
+  </si>
+  <si>
+    <t>3.4</t>
+  </si>
+  <si>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>3.6</t>
+  </si>
+  <si>
+    <t>3.7</t>
+  </si>
+  <si>
     <t>Level 4</t>
+  </si>
+  <si>
+    <t>4.1</t>
+  </si>
+  <si>
+    <t>4.2</t>
+  </si>
+  <si>
+    <t>4.3</t>
+  </si>
+  <si>
+    <t>4.4</t>
+  </si>
+  <si>
+    <t>4.5</t>
+  </si>
+  <si>
+    <t>5.1</t>
+  </si>
+  <si>
+    <t>5.2</t>
+  </si>
+  <si>
+    <t>5.3</t>
   </si>
   <si>
     <t>Values</t>
@@ -239,49 +317,863 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1582">
+  <dxfs count="1659">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF71C165"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFAA61A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB11116"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB11116"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF71C165"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFAA61A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB11116"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB11116"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF71C165"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFAA61A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB11116"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB11116"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF71C165"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFAA61A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB11116"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB11116"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF71C165"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFAA61A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB11116"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB11116"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF71C165"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFAA61A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB11116"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB11116"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF71C165"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFAA61A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB11116"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB11116"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF71C165"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFAA61A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB11116"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB11116"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF71C165"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFAA61A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB11116"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB11116"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF71C165"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFAA61A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB11116"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB11116"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF71C165"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFAA61A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB11116"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB11116"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -17306,16 +18198,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.7265625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:20" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -17339,7 +18231,7 @@
       <c r="S1" s="3"/>
       <c r="T1" s="3"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -17361,7 +18253,7 @@
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -17423,7 +18315,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>21</v>
       </c>
@@ -17447,94 +18339,94 @@
       <c r="S4" s="8"/>
       <c r="T4" s="8"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A5" s="4">
-        <v>1.1000000000000001</v>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="P5" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="R5" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="S5" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="T5" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A6" s="4">
-        <v>1.2</v>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
       <c r="L6" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="M6" s="9"/>
       <c r="N6" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="O6" s="9"/>
       <c r="P6" s="9"/>
@@ -17542,12 +18434,12 @@
       <c r="R6" s="9"/>
       <c r="S6" s="9"/>
       <c r="T6" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A7" s="4">
-        <v>1.3</v>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -17560,7 +18452,7 @@
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
       <c r="L7" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="M7" s="9"/>
       <c r="N7" s="9"/>
@@ -17571,9 +18463,9 @@
       <c r="S7" s="9"/>
       <c r="T7" s="9"/>
     </row>
-    <row r="8" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -17595,269 +18487,269 @@
       <c r="S8" s="8"/>
       <c r="T8" s="8"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A9" s="4">
-        <v>2.1</v>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="N9" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="O9" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="P9" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="Q9" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="R9" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="S9" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="T9" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A10" s="4">
-        <v>2.2000000000000002</v>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="L10" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="M10" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="N10" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="O10" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="P10" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="Q10" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="R10" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="S10" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="T10" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A11" s="4">
-        <v>2.2999999999999998</v>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="J11" s="9"/>
       <c r="K11" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="L11" s="9"/>
       <c r="M11" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="O11" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="P11" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="Q11" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="R11" s="9"/>
       <c r="S11" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="T11" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A12" s="4">
-        <v>2.4</v>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="G12" s="9"/>
       <c r="H12" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
       <c r="L12" s="9"/>
       <c r="M12" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="N12" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="O12" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="P12" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="Q12" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="R12" s="9"/>
       <c r="S12" s="9"/>
       <c r="T12" s="9"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A13" s="4">
-        <v>2.5</v>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
       <c r="M13" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="N13" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="O13" s="9"/>
       <c r="P13" s="9"/>
       <c r="Q13" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="R13" s="9"/>
       <c r="S13" s="9"/>
       <c r="T13" s="9"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A14" s="4">
-        <v>2.6</v>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
@@ -17865,29 +18757,27 @@
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
       <c r="I14" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
       <c r="L14" s="9"/>
       <c r="M14" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="O14" s="9"/>
       <c r="P14" s="9"/>
-      <c r="Q14" s="9" t="s">
-        <v>34</v>
-      </c>
+      <c r="Q14" s="9"/>
       <c r="R14" s="9"/>
       <c r="S14" s="9"/>
       <c r="T14" s="9"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A15" s="4">
-        <v>2.7</v>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
@@ -17902,7 +18792,7 @@
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
       <c r="N15" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="O15" s="9"/>
       <c r="P15" s="9"/>
@@ -17911,9 +18801,9 @@
       <c r="S15" s="9"/>
       <c r="T15" s="9"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A16" s="4">
-        <v>2.8</v>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
@@ -17928,7 +18818,7 @@
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
       <c r="N16" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="O16" s="9"/>
       <c r="P16" s="9"/>
@@ -17937,9 +18827,9 @@
       <c r="S16" s="9"/>
       <c r="T16" s="9"/>
     </row>
-    <row r="17" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -17961,174 +18851,174 @@
       <c r="S17" s="8"/>
       <c r="T17" s="8"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A18" s="4">
-        <v>3.1</v>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="L18" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="M18" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="N18" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="O18" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="P18" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="Q18" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="R18" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="S18" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="T18" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A19" s="4">
-        <v>3.2</v>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="L19" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="M19" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="O19" s="9"/>
       <c r="P19" s="9"/>
       <c r="Q19" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="R19" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="S19" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="T19" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A20" s="4">
-        <v>3.3</v>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="K20" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="L20" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="M20" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="N20" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="O20" s="9"/>
       <c r="P20" s="9"/>
       <c r="Q20" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="R20" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="S20" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="T20" s="9"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A21" s="4">
-        <v>3.4</v>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
@@ -18136,43 +19026,43 @@
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
       <c r="H21" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="J21" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="K21" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="L21" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="M21" s="9"/>
       <c r="N21" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="O21" s="9"/>
       <c r="P21" s="9"/>
       <c r="Q21" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="R21" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="S21" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="T21" s="9"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A22" s="4">
-        <v>3.5</v>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
@@ -18181,35 +19071,35 @@
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="J22" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="K22" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="L22" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="M22" s="9"/>
       <c r="N22" s="9"/>
       <c r="O22" s="9"/>
       <c r="P22" s="9"/>
       <c r="Q22" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="R22" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="S22" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="T22" s="9"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A23" s="4">
-        <v>3.6</v>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -18219,33 +19109,33 @@
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="J23" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="K23" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="L23" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="M23" s="9"/>
       <c r="N23" s="9"/>
       <c r="O23" s="9"/>
       <c r="P23" s="9"/>
       <c r="Q23" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="R23" s="9"/>
       <c r="S23" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="T23" s="9"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A24" s="4">
-        <v>3.7</v>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -18256,24 +19146,22 @@
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
       <c r="J24" s="9"/>
-      <c r="K24" s="9" t="s">
-        <v>34</v>
-      </c>
+      <c r="K24" s="9"/>
       <c r="L24" s="9"/>
       <c r="M24" s="9"/>
       <c r="N24" s="9"/>
       <c r="O24" s="9"/>
       <c r="P24" s="9"/>
       <c r="Q24" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="R24" s="9"/>
       <c r="S24" s="9"/>
       <c r="T24" s="9"/>
     </row>
-    <row r="25" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -18295,32 +19183,34 @@
       <c r="S25" s="8"/>
       <c r="T25" s="8"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A26" s="4">
-        <v>4.0999999999999996</v>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
       <c r="F26" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G26" s="9"/>
+        <v>60</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="H26" s="9"/>
       <c r="I26" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
       <c r="L26" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="M26" s="9"/>
       <c r="N26" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="O26" s="9"/>
       <c r="P26" s="9"/>
@@ -18329,12 +19219,12 @@
       <c r="S26" s="9"/>
       <c r="T26" s="9"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A27" s="4">
-        <v>4.2</v>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
@@ -18343,7 +19233,7 @@
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
       <c r="I27" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="J27" s="9"/>
       <c r="K27" s="9"/>
@@ -18357,9 +19247,9 @@
       <c r="S27" s="9"/>
       <c r="T27" s="9"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A28" s="4">
-        <v>4.3</v>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
@@ -18369,7 +19259,7 @@
       <c r="G28" s="9"/>
       <c r="H28" s="9"/>
       <c r="I28" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
@@ -18383,9 +19273,9 @@
       <c r="S28" s="9"/>
       <c r="T28" s="9"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A29" s="4">
-        <v>4.4000000000000004</v>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -18395,7 +19285,7 @@
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
       <c r="I29" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="J29" s="9"/>
       <c r="K29" s="9"/>
@@ -18409,9 +19299,9 @@
       <c r="S29" s="9"/>
       <c r="T29" s="9"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A30" s="4">
-        <v>4.5</v>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
@@ -18421,7 +19311,7 @@
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
       <c r="I30" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
@@ -18435,7 +19325,7 @@
       <c r="S30" s="9"/>
       <c r="T30" s="9"/>
     </row>
-    <row r="31" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>0</v>
       </c>
@@ -18459,12 +19349,12 @@
       <c r="S31" s="8"/>
       <c r="T31" s="8"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A32" s="4">
-        <v>5.0999999999999996</v>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
@@ -18473,7 +19363,7 @@
       <c r="G32" s="9"/>
       <c r="H32" s="9"/>
       <c r="I32" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
@@ -18487,9 +19377,9 @@
       <c r="S32" s="9"/>
       <c r="T32" s="9"/>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A33" s="4">
-        <v>5.2</v>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>
@@ -18499,7 +19389,7 @@
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
       <c r="I33" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
@@ -18513,9 +19403,9 @@
       <c r="S33" s="9"/>
       <c r="T33" s="9"/>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A34" s="4">
-        <v>5.3</v>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
@@ -18525,7 +19415,7 @@
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
       <c r="I34" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
@@ -18541,926 +19431,1271 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B5">
-    <cfRule type="cellIs" dxfId="1581" priority="281" operator="equal">
+    <cfRule type="cellIs" dxfId="1658" priority="358" operator="equal">
       <formula>"NY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1580" priority="282" operator="equal">
+    <cfRule type="cellIs" dxfId="1657" priority="359" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1579" priority="283" operator="equal">
+    <cfRule type="cellIs" dxfId="1656" priority="360" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1578" priority="284" operator="equal">
+    <cfRule type="cellIs" dxfId="1655" priority="361" operator="equal">
       <formula>"LM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1577" priority="285" operator="equal">
+    <cfRule type="cellIs" dxfId="1654" priority="362" operator="equal">
       <formula>"FM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1576" priority="286" operator="equal">
+    <cfRule type="cellIs" dxfId="1653" priority="363" operator="equal">
       <formula>"NC"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="1575" priority="287">
+    <cfRule type="containsBlanks" dxfId="1652" priority="364">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C5:K5 M5:T5">
-    <cfRule type="cellIs" dxfId="279" priority="274" operator="equal">
+  <conditionalFormatting sqref="C5">
+    <cfRule type="cellIs" dxfId="1651" priority="365" operator="equal">
       <formula>"NY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="278" priority="275" operator="equal">
+    <cfRule type="cellIs" dxfId="1650" priority="366" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="277" priority="276" operator="equal">
+    <cfRule type="cellIs" dxfId="1649" priority="367" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="276" priority="277" operator="equal">
+    <cfRule type="cellIs" dxfId="1648" priority="368" operator="equal">
       <formula>"LM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="275" priority="278" operator="equal">
+    <cfRule type="cellIs" dxfId="1647" priority="369" operator="equal">
       <formula>"FM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="274" priority="279" operator="equal">
+    <cfRule type="cellIs" dxfId="1646" priority="370" operator="equal">
       <formula>"NC"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="273" priority="280">
+    <cfRule type="containsBlanks" dxfId="1645" priority="371">
       <formula>LEN(TRIM(C5))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5">
+    <cfRule type="cellIs" dxfId="1644" priority="372" operator="equal">
+      <formula>"NY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1643" priority="373" operator="equal">
+      <formula>"DM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1642" priority="374" operator="equal">
+      <formula>"PM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1641" priority="375" operator="equal">
+      <formula>"LM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1640" priority="376" operator="equal">
+      <formula>"FM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1639" priority="377" operator="equal">
+      <formula>"NC"</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="1638" priority="378">
+      <formula>LEN(TRIM(D5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="272" priority="267" operator="equal">
+    <cfRule type="cellIs" dxfId="1637" priority="379" operator="equal">
       <formula>"NY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="271" priority="268" operator="equal">
+    <cfRule type="cellIs" dxfId="1636" priority="380" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="270" priority="269" operator="equal">
+    <cfRule type="cellIs" dxfId="1635" priority="381" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="269" priority="270" operator="equal">
+    <cfRule type="cellIs" dxfId="1634" priority="382" operator="equal">
       <formula>"LM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="268" priority="271" operator="equal">
+    <cfRule type="cellIs" dxfId="1633" priority="383" operator="equal">
       <formula>"FM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="267" priority="272" operator="equal">
+    <cfRule type="cellIs" dxfId="1632" priority="384" operator="equal">
       <formula>"NC"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="266" priority="273">
+    <cfRule type="containsBlanks" dxfId="1631" priority="385">
       <formula>LEN(TRIM(D6))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H6:I6">
-    <cfRule type="cellIs" dxfId="265" priority="260" operator="equal">
+  <conditionalFormatting sqref="E5:H5">
+    <cfRule type="cellIs" dxfId="1630" priority="386" operator="equal">
       <formula>"NY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="264" priority="261" operator="equal">
+    <cfRule type="cellIs" dxfId="1629" priority="387" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="263" priority="262" operator="equal">
+    <cfRule type="cellIs" dxfId="1628" priority="388" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="262" priority="263" operator="equal">
+    <cfRule type="cellIs" dxfId="1627" priority="389" operator="equal">
       <formula>"LM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="261" priority="264" operator="equal">
+    <cfRule type="cellIs" dxfId="1626" priority="390" operator="equal">
       <formula>"FM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="260" priority="265" operator="equal">
+    <cfRule type="cellIs" dxfId="1625" priority="391" operator="equal">
       <formula>"NC"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="259" priority="266">
+    <cfRule type="containsBlanks" dxfId="1624" priority="392">
+      <formula>LEN(TRIM(E5))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H6">
+    <cfRule type="cellIs" dxfId="363" priority="351" operator="equal">
+      <formula>"NY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="362" priority="352" operator="equal">
+      <formula>"DM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="361" priority="353" operator="equal">
+      <formula>"PM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="360" priority="354" operator="equal">
+      <formula>"LM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="359" priority="355" operator="equal">
+      <formula>"FM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="358" priority="356" operator="equal">
+      <formula>"NC"</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="357" priority="357">
       <formula>LEN(TRIM(H6))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L5:L7">
-    <cfRule type="cellIs" dxfId="258" priority="253" operator="equal">
+  <conditionalFormatting sqref="I5:I6">
+    <cfRule type="cellIs" dxfId="356" priority="344" operator="equal">
       <formula>"NY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="257" priority="254" operator="equal">
+    <cfRule type="cellIs" dxfId="355" priority="345" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="256" priority="255" operator="equal">
+    <cfRule type="cellIs" dxfId="354" priority="346" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="255" priority="256" operator="equal">
+    <cfRule type="cellIs" dxfId="353" priority="347" operator="equal">
       <formula>"LM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="254" priority="257" operator="equal">
+    <cfRule type="cellIs" dxfId="352" priority="348" operator="equal">
       <formula>"FM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="253" priority="258" operator="equal">
+    <cfRule type="cellIs" dxfId="351" priority="349" operator="equal">
       <formula>"NC"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="252" priority="259">
+    <cfRule type="containsBlanks" dxfId="350" priority="350">
+      <formula>LEN(TRIM(I5))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J5">
+    <cfRule type="cellIs" dxfId="349" priority="337" operator="equal">
+      <formula>"NY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="348" priority="338" operator="equal">
+      <formula>"DM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="347" priority="339" operator="equal">
+      <formula>"PM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="346" priority="340" operator="equal">
+      <formula>"LM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="345" priority="341" operator="equal">
+      <formula>"FM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="344" priority="342" operator="equal">
+      <formula>"NC"</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="343" priority="343">
+      <formula>LEN(TRIM(J5))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K5">
+    <cfRule type="cellIs" dxfId="342" priority="330" operator="equal">
+      <formula>"NY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="341" priority="331" operator="equal">
+      <formula>"DM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="340" priority="332" operator="equal">
+      <formula>"PM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="339" priority="333" operator="equal">
+      <formula>"LM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="338" priority="334" operator="equal">
+      <formula>"FM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="337" priority="335" operator="equal">
+      <formula>"NC"</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="336" priority="336">
+      <formula>LEN(TRIM(K5))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L5">
+    <cfRule type="cellIs" dxfId="335" priority="323" operator="equal">
+      <formula>"NY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="334" priority="324" operator="equal">
+      <formula>"DM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="333" priority="325" operator="equal">
+      <formula>"PM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="332" priority="326" operator="equal">
+      <formula>"LM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="331" priority="327" operator="equal">
+      <formula>"FM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="330" priority="328" operator="equal">
+      <formula>"NC"</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="329" priority="329">
       <formula>LEN(TRIM(L5))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L6">
+    <cfRule type="cellIs" dxfId="328" priority="316" operator="equal">
+      <formula>"NY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="327" priority="317" operator="equal">
+      <formula>"DM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="326" priority="318" operator="equal">
+      <formula>"PM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="325" priority="319" operator="equal">
+      <formula>"LM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="324" priority="320" operator="equal">
+      <formula>"FM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="323" priority="321" operator="equal">
+      <formula>"NC"</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="322" priority="322">
+      <formula>LEN(TRIM(L6))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L7">
+    <cfRule type="cellIs" dxfId="321" priority="309" operator="equal">
+      <formula>"NY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="320" priority="310" operator="equal">
+      <formula>"DM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="319" priority="311" operator="equal">
+      <formula>"PM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="318" priority="312" operator="equal">
+      <formula>"LM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="317" priority="313" operator="equal">
+      <formula>"FM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="316" priority="314" operator="equal">
+      <formula>"NC"</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="315" priority="315">
+      <formula>LEN(TRIM(L7))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M5">
+    <cfRule type="cellIs" dxfId="314" priority="302" operator="equal">
+      <formula>"NY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="313" priority="303" operator="equal">
+      <formula>"DM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="312" priority="304" operator="equal">
+      <formula>"PM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="311" priority="305" operator="equal">
+      <formula>"LM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="310" priority="306" operator="equal">
+      <formula>"FM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="309" priority="307" operator="equal">
+      <formula>"NC"</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="308" priority="308">
+      <formula>LEN(TRIM(M5))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N5">
+    <cfRule type="cellIs" dxfId="307" priority="295" operator="equal">
+      <formula>"NY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="306" priority="296" operator="equal">
+      <formula>"DM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="305" priority="297" operator="equal">
+      <formula>"PM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="304" priority="298" operator="equal">
+      <formula>"LM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="303" priority="299" operator="equal">
+      <formula>"FM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="302" priority="300" operator="equal">
+      <formula>"NC"</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="301" priority="301">
+      <formula>LEN(TRIM(N5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N6">
-    <cfRule type="cellIs" dxfId="251" priority="246" operator="equal">
+    <cfRule type="cellIs" dxfId="300" priority="288" operator="equal">
       <formula>"NY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="250" priority="247" operator="equal">
+    <cfRule type="cellIs" dxfId="299" priority="289" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="249" priority="248" operator="equal">
+    <cfRule type="cellIs" dxfId="298" priority="290" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="248" priority="249" operator="equal">
+    <cfRule type="cellIs" dxfId="297" priority="291" operator="equal">
       <formula>"LM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="247" priority="250" operator="equal">
+    <cfRule type="cellIs" dxfId="296" priority="292" operator="equal">
       <formula>"FM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="246" priority="251" operator="equal">
+    <cfRule type="cellIs" dxfId="295" priority="293" operator="equal">
       <formula>"NC"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="245" priority="252">
+    <cfRule type="containsBlanks" dxfId="294" priority="294">
       <formula>LEN(TRIM(N6))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O5">
+    <cfRule type="cellIs" dxfId="293" priority="281" operator="equal">
+      <formula>"NY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="292" priority="282" operator="equal">
+      <formula>"DM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="291" priority="283" operator="equal">
+      <formula>"PM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="290" priority="284" operator="equal">
+      <formula>"LM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="289" priority="285" operator="equal">
+      <formula>"FM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="288" priority="286" operator="equal">
+      <formula>"NC"</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="287" priority="287">
+      <formula>LEN(TRIM(O5))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P5">
+    <cfRule type="cellIs" dxfId="286" priority="274" operator="equal">
+      <formula>"NY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="285" priority="275" operator="equal">
+      <formula>"DM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="284" priority="276" operator="equal">
+      <formula>"PM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="283" priority="277" operator="equal">
+      <formula>"LM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="282" priority="278" operator="equal">
+      <formula>"FM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="281" priority="279" operator="equal">
+      <formula>"NC"</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="280" priority="280">
+      <formula>LEN(TRIM(P5))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q5">
+    <cfRule type="cellIs" dxfId="279" priority="267" operator="equal">
+      <formula>"NY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="278" priority="268" operator="equal">
+      <formula>"DM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="277" priority="269" operator="equal">
+      <formula>"PM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="276" priority="270" operator="equal">
+      <formula>"LM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="275" priority="271" operator="equal">
+      <formula>"FM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="274" priority="272" operator="equal">
+      <formula>"NC"</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="273" priority="273">
+      <formula>LEN(TRIM(Q5))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R5">
+    <cfRule type="cellIs" dxfId="272" priority="260" operator="equal">
+      <formula>"NY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="271" priority="261" operator="equal">
+      <formula>"DM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="270" priority="262" operator="equal">
+      <formula>"PM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="269" priority="263" operator="equal">
+      <formula>"LM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="268" priority="264" operator="equal">
+      <formula>"FM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="267" priority="265" operator="equal">
+      <formula>"NC"</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="266" priority="266">
+      <formula>LEN(TRIM(R5))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S5">
+    <cfRule type="cellIs" dxfId="265" priority="253" operator="equal">
+      <formula>"NY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="264" priority="254" operator="equal">
+      <formula>"DM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="263" priority="255" operator="equal">
+      <formula>"PM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="262" priority="256" operator="equal">
+      <formula>"LM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="261" priority="257" operator="equal">
+      <formula>"FM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="260" priority="258" operator="equal">
+      <formula>"NC"</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="259" priority="259">
+      <formula>LEN(TRIM(S5))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T5">
+    <cfRule type="cellIs" dxfId="258" priority="246" operator="equal">
+      <formula>"NY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="257" priority="247" operator="equal">
+      <formula>"DM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="256" priority="248" operator="equal">
+      <formula>"PM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="255" priority="249" operator="equal">
+      <formula>"LM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="254" priority="250" operator="equal">
+      <formula>"FM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="253" priority="251" operator="equal">
+      <formula>"NC"</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="252" priority="252">
+      <formula>LEN(TRIM(T5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T6">
-    <cfRule type="cellIs" dxfId="244" priority="239" operator="equal">
+    <cfRule type="cellIs" dxfId="251" priority="239" operator="equal">
       <formula>"NY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="243" priority="240" operator="equal">
+    <cfRule type="cellIs" dxfId="250" priority="240" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="242" priority="241" operator="equal">
+    <cfRule type="cellIs" dxfId="249" priority="241" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="241" priority="242" operator="equal">
+    <cfRule type="cellIs" dxfId="248" priority="242" operator="equal">
       <formula>"LM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="240" priority="243" operator="equal">
+    <cfRule type="cellIs" dxfId="247" priority="243" operator="equal">
       <formula>"FM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="239" priority="244" operator="equal">
+    <cfRule type="cellIs" dxfId="246" priority="244" operator="equal">
       <formula>"NC"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="238" priority="245">
+    <cfRule type="containsBlanks" dxfId="245" priority="245">
       <formula>LEN(TRIM(T6))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B9:T9">
-    <cfRule type="cellIs" dxfId="237" priority="232" operator="equal">
+  <conditionalFormatting sqref="S9:T11">
+    <cfRule type="cellIs" dxfId="244" priority="232" operator="equal">
       <formula>"NY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="236" priority="233" operator="equal">
+    <cfRule type="cellIs" dxfId="243" priority="233" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="235" priority="234" operator="equal">
+    <cfRule type="cellIs" dxfId="242" priority="234" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="234" priority="235" operator="equal">
+    <cfRule type="cellIs" dxfId="241" priority="235" operator="equal">
       <formula>"LM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="233" priority="236" operator="equal">
+    <cfRule type="cellIs" dxfId="240" priority="236" operator="equal">
       <formula>"FM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="232" priority="237" operator="equal">
+    <cfRule type="cellIs" dxfId="239" priority="237" operator="equal">
       <formula>"NC"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="231" priority="238">
+    <cfRule type="containsBlanks" dxfId="238" priority="238">
+      <formula>LEN(TRIM(S9))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9:R10">
+    <cfRule type="cellIs" dxfId="237" priority="225" operator="equal">
+      <formula>"NY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="236" priority="226" operator="equal">
+      <formula>"DM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="235" priority="227" operator="equal">
+      <formula>"PM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="234" priority="228" operator="equal">
+      <formula>"LM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="233" priority="229" operator="equal">
+      <formula>"FM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="232" priority="230" operator="equal">
+      <formula>"NC"</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="231" priority="231">
       <formula>LEN(TRIM(B9))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B10:T10">
-    <cfRule type="cellIs" dxfId="230" priority="225" operator="equal">
+  <conditionalFormatting sqref="C11:D13">
+    <cfRule type="cellIs" dxfId="230" priority="218" operator="equal">
       <formula>"NY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="229" priority="226" operator="equal">
+    <cfRule type="cellIs" dxfId="229" priority="219" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="228" priority="227" operator="equal">
+    <cfRule type="cellIs" dxfId="228" priority="220" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="227" priority="228" operator="equal">
+    <cfRule type="cellIs" dxfId="227" priority="221" operator="equal">
       <formula>"LM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="226" priority="229" operator="equal">
+    <cfRule type="cellIs" dxfId="226" priority="222" operator="equal">
       <formula>"FM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="225" priority="230" operator="equal">
+    <cfRule type="cellIs" dxfId="225" priority="223" operator="equal">
       <formula>"NC"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="224" priority="231">
-      <formula>LEN(TRIM(B10))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C11:F11">
-    <cfRule type="cellIs" dxfId="223" priority="218" operator="equal">
-      <formula>"NY"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="222" priority="219" operator="equal">
-      <formula>"DM"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="221" priority="220" operator="equal">
-      <formula>"PM"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="220" priority="221" operator="equal">
-      <formula>"LM"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="219" priority="222" operator="equal">
-      <formula>"FM"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="218" priority="223" operator="equal">
-      <formula>"NC"</formula>
-    </cfRule>
-    <cfRule type="containsBlanks" dxfId="217" priority="224">
+    <cfRule type="containsBlanks" dxfId="224" priority="224">
       <formula>LEN(TRIM(C11))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C12:D12">
-    <cfRule type="cellIs" dxfId="216" priority="211" operator="equal">
-      <formula>"NY"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="215" priority="212" operator="equal">
-      <formula>"DM"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="214" priority="213" operator="equal">
-      <formula>"PM"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="213" priority="214" operator="equal">
-      <formula>"LM"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="212" priority="215" operator="equal">
-      <formula>"FM"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="211" priority="216" operator="equal">
-      <formula>"NC"</formula>
-    </cfRule>
-    <cfRule type="containsBlanks" dxfId="210" priority="217">
-      <formula>LEN(TRIM(C12))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C13:D13">
-    <cfRule type="cellIs" dxfId="209" priority="204" operator="equal">
-      <formula>"NY"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="208" priority="205" operator="equal">
-      <formula>"DM"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="207" priority="206" operator="equal">
-      <formula>"PM"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="206" priority="207" operator="equal">
-      <formula>"LM"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="205" priority="208" operator="equal">
-      <formula>"FM"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="204" priority="209" operator="equal">
-      <formula>"NC"</formula>
-    </cfRule>
-    <cfRule type="containsBlanks" dxfId="203" priority="210">
-      <formula>LEN(TRIM(C13))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="cellIs" dxfId="202" priority="197" operator="equal">
+    <cfRule type="cellIs" dxfId="223" priority="211" operator="equal">
       <formula>"NY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="201" priority="198" operator="equal">
+    <cfRule type="cellIs" dxfId="222" priority="212" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="200" priority="199" operator="equal">
+    <cfRule type="cellIs" dxfId="221" priority="213" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="199" priority="200" operator="equal">
+    <cfRule type="cellIs" dxfId="220" priority="214" operator="equal">
       <formula>"LM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="198" priority="201" operator="equal">
+    <cfRule type="cellIs" dxfId="219" priority="215" operator="equal">
       <formula>"FM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="197" priority="202" operator="equal">
+    <cfRule type="cellIs" dxfId="218" priority="216" operator="equal">
       <formula>"NC"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="196" priority="203">
+    <cfRule type="containsBlanks" dxfId="217" priority="217">
       <formula>LEN(TRIM(C14))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11:F11">
+    <cfRule type="cellIs" dxfId="216" priority="204" operator="equal">
+      <formula>"NY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="215" priority="205" operator="equal">
+      <formula>"DM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="214" priority="206" operator="equal">
+      <formula>"PM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="213" priority="207" operator="equal">
+      <formula>"LM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="212" priority="208" operator="equal">
+      <formula>"FM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="211" priority="209" operator="equal">
+      <formula>"NC"</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="210" priority="210">
+      <formula>LEN(TRIM(E11))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="cellIs" dxfId="195" priority="190" operator="equal">
+    <cfRule type="cellIs" dxfId="209" priority="197" operator="equal">
       <formula>"NY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="194" priority="191" operator="equal">
+    <cfRule type="cellIs" dxfId="208" priority="198" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="193" priority="192" operator="equal">
+    <cfRule type="cellIs" dxfId="207" priority="199" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="192" priority="193" operator="equal">
+    <cfRule type="cellIs" dxfId="206" priority="200" operator="equal">
       <formula>"LM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="191" priority="194" operator="equal">
+    <cfRule type="cellIs" dxfId="205" priority="201" operator="equal">
       <formula>"FM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="190" priority="195" operator="equal">
+    <cfRule type="cellIs" dxfId="204" priority="202" operator="equal">
       <formula>"NC"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="189" priority="196">
+    <cfRule type="containsBlanks" dxfId="203" priority="203">
       <formula>LEN(TRIM(F12))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11:I12">
-    <cfRule type="cellIs" dxfId="188" priority="183" operator="equal">
+    <cfRule type="cellIs" dxfId="202" priority="190" operator="equal">
       <formula>"NY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="187" priority="184" operator="equal">
+    <cfRule type="cellIs" dxfId="201" priority="191" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="186" priority="185" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="192" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="185" priority="186" operator="equal">
+    <cfRule type="cellIs" dxfId="199" priority="193" operator="equal">
       <formula>"LM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="184" priority="187" operator="equal">
+    <cfRule type="cellIs" dxfId="198" priority="194" operator="equal">
       <formula>"FM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="183" priority="188" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="195" operator="equal">
       <formula>"NC"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="182" priority="189">
+    <cfRule type="containsBlanks" dxfId="196" priority="196">
       <formula>LEN(TRIM(H11))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13:I14">
-    <cfRule type="cellIs" dxfId="181" priority="176" operator="equal">
+    <cfRule type="cellIs" dxfId="195" priority="183" operator="equal">
       <formula>"NY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="180" priority="177" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="184" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="179" priority="178" operator="equal">
+    <cfRule type="cellIs" dxfId="193" priority="185" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="178" priority="179" operator="equal">
+    <cfRule type="cellIs" dxfId="192" priority="186" operator="equal">
       <formula>"LM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="177" priority="180" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="187" operator="equal">
       <formula>"FM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="176" priority="181" operator="equal">
+    <cfRule type="cellIs" dxfId="190" priority="188" operator="equal">
       <formula>"NC"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="175" priority="182">
+    <cfRule type="containsBlanks" dxfId="189" priority="189">
       <formula>LEN(TRIM(I13))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11">
-    <cfRule type="cellIs" dxfId="174" priority="169" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="176" operator="equal">
       <formula>"NY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="173" priority="170" operator="equal">
+    <cfRule type="cellIs" dxfId="187" priority="177" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="172" priority="171" operator="equal">
+    <cfRule type="cellIs" dxfId="186" priority="178" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="171" priority="172" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="179" operator="equal">
       <formula>"LM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="170" priority="173" operator="equal">
+    <cfRule type="cellIs" dxfId="184" priority="180" operator="equal">
       <formula>"FM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="169" priority="174" operator="equal">
+    <cfRule type="cellIs" dxfId="183" priority="181" operator="equal">
       <formula>"NC"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="168" priority="175">
+    <cfRule type="containsBlanks" dxfId="182" priority="182">
       <formula>LEN(TRIM(K11))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M11:Q12">
-    <cfRule type="cellIs" dxfId="167" priority="162" operator="equal">
+    <cfRule type="cellIs" dxfId="181" priority="169" operator="equal">
       <formula>"NY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="166" priority="163" operator="equal">
+    <cfRule type="cellIs" dxfId="180" priority="170" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="165" priority="164" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="171" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="164" priority="165" operator="equal">
+    <cfRule type="cellIs" dxfId="178" priority="172" operator="equal">
       <formula>"LM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="163" priority="166" operator="equal">
+    <cfRule type="cellIs" dxfId="177" priority="173" operator="equal">
       <formula>"FM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="162" priority="167" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="174" operator="equal">
       <formula>"NC"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="161" priority="168">
+    <cfRule type="containsBlanks" dxfId="175" priority="175">
       <formula>LEN(TRIM(M11))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M13:N14">
-    <cfRule type="cellIs" dxfId="160" priority="155" operator="equal">
+    <cfRule type="cellIs" dxfId="174" priority="162" operator="equal">
       <formula>"NY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="159" priority="156" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="163" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="158" priority="157" operator="equal">
+    <cfRule type="cellIs" dxfId="172" priority="164" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="157" priority="158" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="165" operator="equal">
       <formula>"LM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="156" priority="159" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="166" operator="equal">
       <formula>"FM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="155" priority="160" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="167" operator="equal">
       <formula>"NC"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="154" priority="161">
+    <cfRule type="containsBlanks" dxfId="168" priority="168">
       <formula>LEN(TRIM(M13))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N15:N16">
-    <cfRule type="cellIs" dxfId="153" priority="148" operator="equal">
+  <conditionalFormatting sqref="N15">
+    <cfRule type="cellIs" dxfId="167" priority="155" operator="equal">
       <formula>"NY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="152" priority="149" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="156" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="151" priority="150" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="157" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="150" priority="151" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="158" operator="equal">
       <formula>"LM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="149" priority="152" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="159" operator="equal">
       <formula>"FM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="148" priority="153" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="160" operator="equal">
       <formula>"NC"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="147" priority="154">
+    <cfRule type="containsBlanks" dxfId="161" priority="161">
       <formula>LEN(TRIM(N15))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q13:Q14">
-    <cfRule type="cellIs" dxfId="146" priority="141" operator="equal">
+  <conditionalFormatting sqref="N16">
+    <cfRule type="cellIs" dxfId="160" priority="148" operator="equal">
       <formula>"NY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="145" priority="142" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="149" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="143" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="150" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="143" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="151" operator="equal">
       <formula>"LM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="142" priority="145" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="152" operator="equal">
       <formula>"FM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="141" priority="146" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="153" operator="equal">
       <formula>"NC"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="140" priority="147">
+    <cfRule type="containsBlanks" dxfId="154" priority="154">
+      <formula>LEN(TRIM(N16))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q13">
+    <cfRule type="cellIs" dxfId="153" priority="141" operator="equal">
+      <formula>"NY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="152" priority="142" operator="equal">
+      <formula>"DM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="151" priority="143" operator="equal">
+      <formula>"PM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="150" priority="144" operator="equal">
+      <formula>"LM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="149" priority="145" operator="equal">
+      <formula>"FM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="148" priority="146" operator="equal">
+      <formula>"NC"</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="147" priority="147">
       <formula>LEN(TRIM(Q13))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S11:T11">
-    <cfRule type="cellIs" dxfId="139" priority="134" operator="equal">
+  <conditionalFormatting sqref="D18:T18">
+    <cfRule type="cellIs" dxfId="146" priority="134" operator="equal">
       <formula>"NY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="138" priority="135" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="135" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="136" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="136" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="136" priority="137" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="137" operator="equal">
       <formula>"LM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="135" priority="138" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="138" operator="equal">
       <formula>"FM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="134" priority="139" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="139" operator="equal">
       <formula>"NC"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="133" priority="140">
-      <formula>LEN(TRIM(S11))=0</formula>
+    <cfRule type="containsBlanks" dxfId="140" priority="140">
+      <formula>LEN(TRIM(D18))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:B22">
-    <cfRule type="cellIs" dxfId="132" priority="127" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="127" operator="equal">
       <formula>"NY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="131" priority="128" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="128" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="130" priority="129" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="129" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="129" priority="130" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="130" operator="equal">
       <formula>"LM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="131" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="131" operator="equal">
       <formula>"FM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="127" priority="132" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="132" operator="equal">
       <formula>"NC"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="126" priority="133">
+    <cfRule type="containsBlanks" dxfId="133" priority="133">
       <formula>LEN(TRIM(B18))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D18:T18">
-    <cfRule type="cellIs" dxfId="125" priority="120" operator="equal">
-      <formula>"NY"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="124" priority="121" operator="equal">
-      <formula>"DM"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="123" priority="122" operator="equal">
-      <formula>"PM"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="123" operator="equal">
-      <formula>"LM"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="121" priority="124" operator="equal">
-      <formula>"FM"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="125" operator="equal">
-      <formula>"NC"</formula>
-    </cfRule>
-    <cfRule type="containsBlanks" dxfId="119" priority="126">
-      <formula>LEN(TRIM(D18))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19:N19">
-    <cfRule type="cellIs" dxfId="118" priority="113" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="120" operator="equal">
       <formula>"NY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="117" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="121" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="122" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="115" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="123" operator="equal">
       <formula>"LM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="124" operator="equal">
       <formula>"FM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="118" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="125" operator="equal">
       <formula>"NC"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="112" priority="119">
+    <cfRule type="containsBlanks" dxfId="126" priority="126">
       <formula>LEN(TRIM(E19))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G20:N20">
-    <cfRule type="cellIs" dxfId="111" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="113" operator="equal">
       <formula>"NY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="114" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="115" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="116" operator="equal">
       <formula>"LM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="107" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="117" operator="equal">
       <formula>"FM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="118" operator="equal">
       <formula>"NC"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="105" priority="112">
+    <cfRule type="containsBlanks" dxfId="119" priority="119">
       <formula>LEN(TRIM(G20))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21:L21">
-    <cfRule type="cellIs" dxfId="104" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="106" operator="equal">
       <formula>"NY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="107" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="108" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="109" operator="equal">
       <formula>"LM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="110" operator="equal">
       <formula>"FM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="111" operator="equal">
       <formula>"NC"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="98" priority="105">
+    <cfRule type="containsBlanks" dxfId="112" priority="112">
       <formula>LEN(TRIM(H21))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I22:L23">
-    <cfRule type="cellIs" dxfId="97" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="99" operator="equal">
       <formula>"NY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="100" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="101" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="102" operator="equal">
       <formula>"LM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="103" operator="equal">
       <formula>"FM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="104" operator="equal">
       <formula>"NC"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="91" priority="98">
+    <cfRule type="containsBlanks" dxfId="105" priority="105">
       <formula>LEN(TRIM(I22))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K24">
-    <cfRule type="cellIs" dxfId="90" priority="85" operator="equal">
-      <formula>"NY"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="86" operator="equal">
-      <formula>"DM"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="87" operator="equal">
-      <formula>"PM"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="88" operator="equal">
-      <formula>"LM"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="89" operator="equal">
-      <formula>"FM"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="90" operator="equal">
-      <formula>"NC"</formula>
-    </cfRule>
-    <cfRule type="containsBlanks" dxfId="84" priority="91">
-      <formula>LEN(TRIM(K24))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N21">
-    <cfRule type="cellIs" dxfId="83" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="92" operator="equal">
       <formula>"NY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="93" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="94" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="95" operator="equal">
       <formula>"LM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="96" operator="equal">
       <formula>"FM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="97" operator="equal">
       <formula>"NC"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="77" priority="84">
+    <cfRule type="containsBlanks" dxfId="98" priority="98">
       <formula>LEN(TRIM(N21))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q19:S22">
-    <cfRule type="cellIs" dxfId="76" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="85" operator="equal">
       <formula>"NY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="86" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="87" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="88" operator="equal">
       <formula>"LM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="89" operator="equal">
       <formula>"FM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="90" operator="equal">
       <formula>"NC"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="70" priority="77">
+    <cfRule type="containsBlanks" dxfId="91" priority="91">
       <formula>LEN(TRIM(Q19))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q23:Q24">
-    <cfRule type="cellIs" dxfId="69" priority="64" operator="equal">
+  <conditionalFormatting sqref="Q23">
+    <cfRule type="cellIs" dxfId="90" priority="78" operator="equal">
       <formula>"NY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="79" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="80" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="81" operator="equal">
       <formula>"LM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="82" operator="equal">
       <formula>"FM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="83" operator="equal">
       <formula>"NC"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="63" priority="70">
+    <cfRule type="containsBlanks" dxfId="84" priority="84">
       <formula>LEN(TRIM(Q23))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q24">
+    <cfRule type="cellIs" dxfId="83" priority="71" operator="equal">
+      <formula>"NY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="82" priority="72" operator="equal">
+      <formula>"DM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="81" priority="73" operator="equal">
+      <formula>"PM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="80" priority="74" operator="equal">
+      <formula>"LM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="79" priority="75" operator="equal">
+      <formula>"FM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="78" priority="76" operator="equal">
+      <formula>"NC"</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="77" priority="77">
+      <formula>LEN(TRIM(Q24))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S23">
-    <cfRule type="cellIs" dxfId="62" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="64" operator="equal">
       <formula>"NY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="65" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="66" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="67" operator="equal">
       <formula>"LM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="68" operator="equal">
       <formula>"FM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="69" operator="equal">
       <formula>"NC"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="56" priority="63">
+    <cfRule type="containsBlanks" dxfId="70" priority="70">
       <formula>LEN(TRIM(S23))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T19">
-    <cfRule type="cellIs" dxfId="55" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="57" operator="equal">
       <formula>"NY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="58" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="59" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="60" operator="equal">
       <formula>"LM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="61" operator="equal">
       <formula>"FM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="62" operator="equal">
       <formula>"NC"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="49" priority="56">
+    <cfRule type="containsBlanks" dxfId="63" priority="63">
       <formula>LEN(TRIM(T19))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B26:B27">
-    <cfRule type="cellIs" dxfId="48" priority="43" operator="equal">
+  <conditionalFormatting sqref="B26">
+    <cfRule type="cellIs" dxfId="62" priority="50" operator="equal">
       <formula>"NY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="51" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="52" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="53" operator="equal">
       <formula>"LM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="54" operator="equal">
       <formula>"FM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="55" operator="equal">
       <formula>"NC"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="42" priority="49">
+    <cfRule type="containsBlanks" dxfId="56" priority="56">
       <formula>LEN(TRIM(B26))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27">
+    <cfRule type="cellIs" dxfId="55" priority="43" operator="equal">
+      <formula>"NY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="44" operator="equal">
+      <formula>"DM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="45" operator="equal">
+      <formula>"PM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="46" operator="equal">
+      <formula>"LM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="51" priority="47" operator="equal">
+      <formula>"FM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="48" operator="equal">
+      <formula>"NC"</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="49" priority="49">
+      <formula>LEN(TRIM(B27))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F26:G26">
+    <cfRule type="cellIs" dxfId="48" priority="36" operator="equal">
+      <formula>"NY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="37" operator="equal">
+      <formula>"DM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="38" operator="equal">
+      <formula>"PM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="39" operator="equal">
+      <formula>"LM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="40" operator="equal">
+      <formula>"FM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="41" operator="equal">
+      <formula>"NC"</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="42" priority="42">
+      <formula>LEN(TRIM(F26))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I26:I30">
+    <cfRule type="cellIs" dxfId="41" priority="29" operator="equal">
+      <formula>"NY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="30" operator="equal">
+      <formula>"DM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="31" operator="equal">
+      <formula>"PM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="32" operator="equal">
+      <formula>"LM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="33" operator="equal">
+      <formula>"FM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="34" operator="equal">
+      <formula>"NC"</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="35" priority="35">
+      <formula>LEN(TRIM(I26))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L26">
+    <cfRule type="cellIs" dxfId="34" priority="22" operator="equal">
+      <formula>"NY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="23" operator="equal">
+      <formula>"DM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="24" operator="equal">
+      <formula>"PM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="25" operator="equal">
+      <formula>"LM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="26" operator="equal">
+      <formula>"FM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="27" operator="equal">
+      <formula>"NC"</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="28" priority="28">
+      <formula>LEN(TRIM(L26))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N26">
+    <cfRule type="cellIs" dxfId="27" priority="15" operator="equal">
+      <formula>"NY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="16" operator="equal">
+      <formula>"DM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="17" operator="equal">
+      <formula>"PM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="18" operator="equal">
+      <formula>"LM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="19" operator="equal">
+      <formula>"FM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="20" operator="equal">
+      <formula>"NC"</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="21" priority="21">
+      <formula>LEN(TRIM(N26))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="cellIs" dxfId="41" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="8" operator="equal">
       <formula>"NY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
       <formula>"LM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="12" operator="equal">
       <formula>"FM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
       <formula>"NC"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="35" priority="42">
+    <cfRule type="containsBlanks" dxfId="14" priority="14">
       <formula>LEN(TRIM(B32))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F26">
-    <cfRule type="cellIs" dxfId="34" priority="29" operator="equal">
-      <formula>"NY"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="30" operator="equal">
-      <formula>"DM"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="31" operator="equal">
-      <formula>"PM"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="32" operator="equal">
-      <formula>"LM"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="33" operator="equal">
-      <formula>"FM"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="34" operator="equal">
-      <formula>"NC"</formula>
-    </cfRule>
-    <cfRule type="containsBlanks" dxfId="28" priority="35">
-      <formula>LEN(TRIM(F26))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I26:I30">
-    <cfRule type="cellIs" dxfId="27" priority="22" operator="equal">
-      <formula>"NY"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="23" operator="equal">
-      <formula>"DM"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="24" operator="equal">
-      <formula>"PM"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="25" operator="equal">
-      <formula>"LM"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="26" operator="equal">
-      <formula>"FM"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="27" operator="equal">
-      <formula>"NC"</formula>
-    </cfRule>
-    <cfRule type="containsBlanks" dxfId="21" priority="28">
-      <formula>LEN(TRIM(I26))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I32:I34">
-    <cfRule type="cellIs" dxfId="20" priority="15" operator="equal">
-      <formula>"NY"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="16" operator="equal">
-      <formula>"DM"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="17" operator="equal">
-      <formula>"PM"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
-      <formula>"LM"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="19" operator="equal">
-      <formula>"FM"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="20" operator="equal">
-      <formula>"NC"</formula>
-    </cfRule>
-    <cfRule type="containsBlanks" dxfId="14" priority="21">
-      <formula>LEN(TRIM(I32))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L26">
-    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
-      <formula>"NY"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
-      <formula>"DM"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
-      <formula>"PM"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
-      <formula>"LM"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
-      <formula>"FM"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="13" operator="equal">
-      <formula>"NC"</formula>
-    </cfRule>
-    <cfRule type="containsBlanks" dxfId="7" priority="14">
-      <formula>LEN(TRIM(L26))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N26">
     <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>"NY"</formula>
     </cfRule>
@@ -19480,11 +20715,11 @@
       <formula>"NC"</formula>
     </cfRule>
     <cfRule type="containsBlanks" dxfId="0" priority="7">
-      <formula>LEN(TRIM(N26))=0</formula>
+      <formula>LEN(TRIM(I32))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I26:I30 Q22:Q24 T5:T6 K10:K11 B18:B22 O5:S5 D5:D6 H6:I6 L6:L7 L10:T10 F11:F12 I12:I14 C11:E11 C13:C14 H12 M12:P12 D13 M14 N5:N6 Q12:Q14 N14:N16 S11:T11 D18:T18 E19:N19 G20:M20 K23:K24 H21:L21 L23 Q19:T19 B32 F26 I32:I34 L26 B26:B27 I23:J23 N20:N21 R22 B5:C5 E5:M5 B9:T9 B10:J10 C12:D12 H11:I11 M11:Q11 M13:N13 I22:L22 S22:S23 Q20:S21 N26" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B32 D6 H6:I6 L5:L7 N5:N6 O5:S5 M5 B10:J10 F11:F12 I12:I14 K10:K11 T5:T6 L10:R10 D11:E11 H12 M12:P12 N14:N16 M14 D18:T18 Q12:Q13 B18:B22 M13:N13 E19:N19 N20:N21 G20:M20 I22:L23 H21:L21 R22 Q22:Q24 Q19:T19 B26:B27 F26:G26 I26:I30 L26 N26 B5:K5 S9:T11 B9:R9 C11:C14 D12:D13 H11:I11 M11:Q11 S22:S23 Q20:S21 I32:I34" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"NY,DM,PM,LM,FM,NC"</formula1>
     </dataValidation>
   </dataValidations>
@@ -19498,66 +20733,325 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" customWidth="1"/>
-    <col min="2" max="2" width="17.26953125" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005FE19CB9C027FD48A4D0D971E52FCFA5" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9e385c74191603dffabceee006c03248">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f366be14-7381-43f6-96f9-9d7bb28bad97" xmlns:ns3="ec500478-62e0-46fc-87f1-cfa988e486b4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="febe07d5ddaa80cb3f86f287337aa8e1" ns2:_="" ns3:_="">
+    <xsd:import namespace="f366be14-7381-43f6-96f9-9d7bb28bad97"/>
+    <xsd:import namespace="ec500478-62e0-46fc-87f1-cfa988e486b4"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="f366be14-7381-43f6-96f9-9d7bb28bad97" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="11" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="15" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="7f35f27a-c890-4130-b78e-bbe546ff31bf" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="17" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="18" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="19" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="20" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="ec500478-62e0-46fc-87f1-cfa988e486b4" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="12" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="13" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="16" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{516b899e-718a-4501-bed1-5bdbb6269459}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="ec500478-62e0-46fc-87f1-cfa988e486b4">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FB7D71E-9AD9-4211-9872-5DD4CE37502F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62374213-EC9A-42E2-9A61-4187ECF45D0A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f366be14-7381-43f6-96f9-9d7bb28bad97"/>
+    <ds:schemaRef ds:uri="ec500478-62e0-46fc-87f1-cfa988e486b4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>